<commit_message>
add 703 about Heap
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289C1840-7784-C34A-9170-D43E065D0764}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB66B138-B04E-8C4D-925F-61FBAD47608B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -91,6 +91,13 @@
   </si>
   <si>
     <t>理解しきれてはない</t>
+    <rPh sb="0" eb="2">
+      <t>リカイ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>理解</t>
     <rPh sb="0" eb="2">
       <t>リカイ</t>
     </rPh>
@@ -533,7 +540,7 @@
   <dimension ref="A1:Z86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -662,6 +669,12 @@
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C12" s="11">
+        <v>44205</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="str">

</xml_diff>

<commit_message>
add 104 about BFS
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB66B138-B04E-8C4D-925F-61FBAD47608B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE70EEA4-1473-5940-B55F-8B301360FA3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -88,13 +88,6 @@
   </si>
   <si>
     <t>Others</t>
-  </si>
-  <si>
-    <t>理解しきれてはない</t>
-    <rPh sb="0" eb="2">
-      <t>リカイ</t>
-    </rPh>
-    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>理解</t>
@@ -103,12 +96,64 @@
     </rPh>
     <phoneticPr fontId="8"/>
   </si>
+  <si>
+    <t>sort, heapqの関数を使えば解ける．アルゴリズムを一から実装はむり．</t>
+    <rPh sb="32" eb="34">
+      <t>ジッソウ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>◎</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>何も見ないで解ける</t>
+    <rPh sb="0" eb="1">
+      <t>ナニ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>◯</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>理解はしてる</t>
+    <rPh sb="0" eb="2">
+      <t>リカイ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>△</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>なんとなく理解</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>わからん</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>有料</t>
+    <rPh sb="0" eb="2">
+      <t>ユウリョ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,6 +202,11 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -192,6 +242,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="56" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -540,7 +592,7 @@
   <dimension ref="A1:Z86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -584,6 +636,18 @@
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
+      <c r="H2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
@@ -594,6 +658,18 @@
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
@@ -614,6 +690,9 @@
         <v>44200</v>
       </c>
       <c r="D5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -673,7 +752,10 @@
         <v>44205</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
@@ -722,6 +804,15 @@
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C16" s="11">
+        <v>44206</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="str">
@@ -753,6 +844,12 @@
       </c>
       <c r="B21" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C21" s="11">
+        <v>44206</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
@@ -1012,6 +1109,9 @@
       <c r="B46" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D46" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="8" t="str">
@@ -1140,8 +1240,12 @@
       <c r="B59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
+      <c r="C59" s="13">
+        <v>44207</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>

</xml_diff>

<commit_message>
add 53 about DP
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE70EEA4-1473-5940-B55F-8B301360FA3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F68E1A-BA91-1B4C-B739-AD558431D86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -165,30 +165,36 @@
       <sz val="18"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -592,7 +598,7 @@
   <dimension ref="A1:Z86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -999,6 +1005,12 @@
       <c r="B35" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C35" s="11">
+        <v>44208</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="str">
@@ -1007,6 +1019,12 @@
       </c>
       <c r="B36" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C36" s="11">
+        <v>44208</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
add 200 about Graph_BFS
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F68E1A-BA91-1B4C-B739-AD558431D86B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206BE201-D6A1-B44A-A413-EEB3F7E98214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1148,6 +1148,12 @@
       <c r="B48" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C48" s="11">
+        <v>44209</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="49" spans="1:26" ht="13">
       <c r="A49" s="8" t="str">

</xml_diff>

<commit_message>
add 50 about recursion
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshi\Desktop\leetcode_study\60probrems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206BE201-D6A1-B44A-A413-EEB3F7E98214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D945DA81-2F11-4BCC-A616-5C713CE7603F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11715" yWindow="1073" windowWidth="1980" windowHeight="6254" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,13 +586,13 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+    <col min="1" max="1" width="50.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -940,6 +929,12 @@
       <c r="B29" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C29" s="11">
+        <v>44210</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="str">
@@ -1140,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="13">
+    <row r="48" spans="1:26" ht="12.75">
       <c r="A48" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/maximum-subarray/","Maximum Subarray")</f>
         <v>Maximum Subarray</v>
@@ -1155,7 +1150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="13">
+    <row r="49" spans="1:26" ht="12.75">
       <c r="A49" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
@@ -1164,7 +1159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="13">
+    <row r="50" spans="1:26" ht="12.75">
       <c r="A50" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/unique-paths-ii/","Unique Paths II")</f>
         <v>Unique Paths II</v>
@@ -1173,7 +1168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="13">
+    <row r="51" spans="1:26" ht="12.75">
       <c r="A51" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/house-robber/","House Robber")</f>
         <v>House Robber</v>
@@ -1182,7 +1177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="13">
+    <row r="52" spans="1:26" ht="12.75">
       <c r="A52" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/house-robber-ii/","House Robber II")</f>
         <v>House Robber II</v>
@@ -1191,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="13">
+    <row r="53" spans="1:26" ht="12.75">
       <c r="A53" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/best-time-to-buy-and-sell-stock/","Best Time to Buy and Sell Stock")</f>
         <v>Best Time to Buy and Sell Stock</v>
@@ -1200,7 +1195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="13">
+    <row r="54" spans="1:26" ht="12.75">
       <c r="A54" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/","Best Time to Buy and Sell Stock II")</f>
         <v>Best Time to Buy and Sell Stock II</v>
@@ -1209,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="13">
+    <row r="55" spans="1:26" ht="12.75">
       <c r="A55" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/word-break/","Word Break")</f>
         <v>Word Break</v>
@@ -1242,7 +1237,7 @@
       <c r="Y55" s="10"/>
       <c r="Z55" s="10"/>
     </row>
-    <row r="56" spans="1:26" ht="13">
+    <row r="56" spans="1:26" ht="12.75">
       <c r="A56" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/coin-change/","Coin Change")</f>
         <v>Coin Change</v>
@@ -1251,12 +1246,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="13">
+    <row r="58" spans="1:26" ht="13.15">
       <c r="A58" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="13">
+    <row r="59" spans="1:26" ht="12.75">
       <c r="A59" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/search-insert-position/","Search Insert Position")</f>
         <v>Search Insert Position</v>
@@ -1293,7 +1288,7 @@
       <c r="Y59" s="10"/>
       <c r="Z59" s="10"/>
     </row>
-    <row r="60" spans="1:26" ht="13">
+    <row r="60" spans="1:26" ht="12.75">
       <c r="A60" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/","Find Minimum in Rotated Sorted Array")</f>
         <v>Find Minimum in Rotated Sorted Array</v>
@@ -1302,7 +1297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="13">
+    <row r="61" spans="1:26" ht="12.75">
       <c r="A61" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/search-in-rotated-sorted-array/","Search in Rotated Sorted Array")</f>
         <v>Search in Rotated Sorted Array</v>
@@ -1311,7 +1306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="13">
+    <row r="62" spans="1:26" ht="12.75">
       <c r="A62" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/capacity-to-ship-packages-within-d-days/","Capacity To Ship Packages Within D Days")</f>
         <v>Capacity To Ship Packages Within D Days</v>
@@ -1320,12 +1315,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="13">
+    <row r="64" spans="1:26" ht="13.15">
       <c r="A64" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="13">
+    <row r="65" spans="1:26" ht="12.75">
       <c r="A65" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/powx-n/","Pow(x, n)")</f>
         <v>Pow(x, n)</v>
@@ -1333,8 +1328,14 @@
       <c r="B65" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" ht="13">
+      <c r="C65" s="11">
+        <v>44211</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" ht="12.75">
       <c r="A66" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/k-th-symbol-in-grammar/","K-th Symbol in Grammar")</f>
         <v>K-th Symbol in Grammar</v>
@@ -1343,7 +1344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="13">
+    <row r="67" spans="1:26" ht="12.75">
       <c r="A67" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/split-bst/","Split BST")</f>
         <v>Split BST</v>
@@ -1352,12 +1353,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="13">
+    <row r="69" spans="1:26" ht="13.15">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="13">
+    <row r="70" spans="1:26" ht="12.75">
       <c r="A70" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/longest-substring-without-repeating-characters/","Longest Substring Without Repeating Characters")</f>
         <v>Longest Substring Without Repeating Characters</v>
@@ -1366,7 +1367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="13">
+    <row r="71" spans="1:26" ht="12.75">
       <c r="A71" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/minimum-size-subarray-sum/","Minimum Size Subarray Sum")</f>
         <v>Minimum Size Subarray Sum</v>
@@ -1375,12 +1376,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="13">
+    <row r="73" spans="1:26" ht="13.15">
       <c r="A73" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="13">
+    <row r="74" spans="1:26" ht="12.75">
       <c r="A74" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/permutations/","Permutations")</f>
         <v>Permutations</v>
@@ -1389,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="13">
+    <row r="75" spans="1:26" ht="12.75">
       <c r="A75" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/subsets/","Subsets")</f>
         <v>Subsets</v>
@@ -1422,7 +1423,7 @@
       <c r="Y75" s="10"/>
       <c r="Z75" s="10"/>
     </row>
-    <row r="76" spans="1:26" ht="13">
+    <row r="76" spans="1:26" ht="12.75">
       <c r="A76" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/combination-sum/","Combination Sum")</f>
         <v>Combination Sum</v>
@@ -1431,7 +1432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="13">
+    <row r="77" spans="1:26" ht="12.75">
       <c r="A77" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/generate-parentheses/","Generate Parentheses")</f>
         <v>Generate Parentheses</v>
@@ -1440,12 +1441,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="13">
+    <row r="79" spans="1:26" ht="13.15">
       <c r="A79" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="13">
+    <row r="80" spans="1:26" ht="12.75">
       <c r="A80" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/move-zeroes/","Move Zeroes")</f>
         <v>Move Zeroes</v>
@@ -1454,7 +1455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="13">
+    <row r="81" spans="1:2" ht="12.75">
       <c r="A81" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/meeting-rooms/","Meeting Rooms")</f>
         <v>Meeting Rooms</v>
@@ -1463,7 +1464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="13">
+    <row r="82" spans="1:2" ht="12.75">
       <c r="A82" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/meeting-rooms-ii/","Meeting Rooms II")</f>
         <v>Meeting Rooms II</v>
@@ -1472,7 +1473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="13">
+    <row r="83" spans="1:2" ht="12.75">
       <c r="A83" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/is-subsequence/","Is Subsequence")</f>
         <v>Is Subsequence</v>
@@ -1481,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="13">
+    <row r="84" spans="1:2" ht="12.75">
       <c r="A84" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/next-permutation/","Next Permutation")</f>
         <v>Next Permutation</v>
@@ -1490,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13">
+    <row r="85" spans="1:2" ht="12.75">
       <c r="A85" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/string-to-integer-atoi/","String to Integer (atoi)")</f>
         <v>String to Integer (atoi)</v>
@@ -1499,7 +1500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="13">
+    <row r="86" spans="1:2" ht="12.75">
       <c r="A86" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/zigzag-conversion/","ZigZag Conversion")</f>
         <v>ZigZag Conversion</v>
@@ -1529,5 +1530,6 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 283 about Others
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshi\Desktop\leetcode_study\60probrems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78B045C-EAE1-5C41-BD42-15862CFF9798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A263C-523A-4573-BF3D-24B84D49B256}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,13 +586,13 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+    <col min="1" max="1" width="50.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -1146,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="13">
+    <row r="48" spans="1:26" ht="12.75">
       <c r="A48" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/maximum-subarray/","Maximum Subarray")</f>
         <v>Maximum Subarray</v>
@@ -1161,7 +1150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="13">
+    <row r="49" spans="1:26" ht="12.75">
       <c r="A49" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
@@ -1170,7 +1159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="13">
+    <row r="50" spans="1:26" ht="12.75">
       <c r="A50" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/unique-paths-ii/","Unique Paths II")</f>
         <v>Unique Paths II</v>
@@ -1179,7 +1168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="13">
+    <row r="51" spans="1:26" ht="12.75">
       <c r="A51" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/house-robber/","House Robber")</f>
         <v>House Robber</v>
@@ -1188,7 +1177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="13">
+    <row r="52" spans="1:26" ht="12.75">
       <c r="A52" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/house-robber-ii/","House Robber II")</f>
         <v>House Robber II</v>
@@ -1197,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="13">
+    <row r="53" spans="1:26" ht="12.75">
       <c r="A53" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/best-time-to-buy-and-sell-stock/","Best Time to Buy and Sell Stock")</f>
         <v>Best Time to Buy and Sell Stock</v>
@@ -1206,7 +1195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="13">
+    <row r="54" spans="1:26" ht="12.75">
       <c r="A54" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/","Best Time to Buy and Sell Stock II")</f>
         <v>Best Time to Buy and Sell Stock II</v>
@@ -1215,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="13">
+    <row r="55" spans="1:26" ht="12.75">
       <c r="A55" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/word-break/","Word Break")</f>
         <v>Word Break</v>
@@ -1248,7 +1237,7 @@
       <c r="Y55" s="10"/>
       <c r="Z55" s="10"/>
     </row>
-    <row r="56" spans="1:26" ht="13">
+    <row r="56" spans="1:26" ht="12.75">
       <c r="A56" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/coin-change/","Coin Change")</f>
         <v>Coin Change</v>
@@ -1257,12 +1246,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="13">
+    <row r="58" spans="1:26" ht="13.15">
       <c r="A58" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="13">
+    <row r="59" spans="1:26" ht="12.75">
       <c r="A59" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/search-insert-position/","Search Insert Position")</f>
         <v>Search Insert Position</v>
@@ -1299,7 +1288,7 @@
       <c r="Y59" s="10"/>
       <c r="Z59" s="10"/>
     </row>
-    <row r="60" spans="1:26" ht="13">
+    <row r="60" spans="1:26" ht="12.75">
       <c r="A60" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/","Find Minimum in Rotated Sorted Array")</f>
         <v>Find Minimum in Rotated Sorted Array</v>
@@ -1308,7 +1297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="13">
+    <row r="61" spans="1:26" ht="12.75">
       <c r="A61" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/search-in-rotated-sorted-array/","Search in Rotated Sorted Array")</f>
         <v>Search in Rotated Sorted Array</v>
@@ -1317,7 +1306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="13">
+    <row r="62" spans="1:26" ht="12.75">
       <c r="A62" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/capacity-to-ship-packages-within-d-days/","Capacity To Ship Packages Within D Days")</f>
         <v>Capacity To Ship Packages Within D Days</v>
@@ -1326,12 +1315,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="13">
+    <row r="64" spans="1:26" ht="13.15">
       <c r="A64" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="13">
+    <row r="65" spans="1:26" ht="12.75">
       <c r="A65" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/powx-n/","Pow(x, n)")</f>
         <v>Pow(x, n)</v>
@@ -1346,7 +1335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="13">
+    <row r="66" spans="1:26" ht="12.75">
       <c r="A66" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/k-th-symbol-in-grammar/","K-th Symbol in Grammar")</f>
         <v>K-th Symbol in Grammar</v>
@@ -1355,7 +1344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="13">
+    <row r="67" spans="1:26" ht="12.75">
       <c r="A67" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/split-bst/","Split BST")</f>
         <v>Split BST</v>
@@ -1364,12 +1353,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="13">
+    <row r="69" spans="1:26" ht="13.15">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="13">
+    <row r="70" spans="1:26" ht="12.75">
       <c r="A70" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/longest-substring-without-repeating-characters/","Longest Substring Without Repeating Characters")</f>
         <v>Longest Substring Without Repeating Characters</v>
@@ -1377,8 +1366,14 @@
       <c r="B70" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" ht="13">
+      <c r="C70" s="11">
+        <v>44213</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="12.75">
       <c r="A71" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/minimum-size-subarray-sum/","Minimum Size Subarray Sum")</f>
         <v>Minimum Size Subarray Sum</v>
@@ -1387,12 +1382,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="13">
+    <row r="73" spans="1:26" ht="13.15">
       <c r="A73" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="13">
+    <row r="74" spans="1:26" ht="12.75">
       <c r="A74" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/permutations/","Permutations")</f>
         <v>Permutations</v>
@@ -1407,7 +1402,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="13">
+    <row r="75" spans="1:26" ht="12.75">
       <c r="A75" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/subsets/","Subsets")</f>
         <v>Subsets</v>
@@ -1439,7 +1434,7 @@
       <c r="Y75" s="10"/>
       <c r="Z75" s="10"/>
     </row>
-    <row r="76" spans="1:26" ht="13">
+    <row r="76" spans="1:26" ht="12.75">
       <c r="A76" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/combination-sum/","Combination Sum")</f>
         <v>Combination Sum</v>
@@ -1448,7 +1443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="13">
+    <row r="77" spans="1:26" ht="12.75">
       <c r="A77" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/generate-parentheses/","Generate Parentheses")</f>
         <v>Generate Parentheses</v>
@@ -1457,12 +1452,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="13">
+    <row r="79" spans="1:26" ht="13.15">
       <c r="A79" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="13">
+    <row r="80" spans="1:26" ht="12.75">
       <c r="A80" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/move-zeroes/","Move Zeroes")</f>
         <v>Move Zeroes</v>
@@ -1470,8 +1465,14 @@
       <c r="B80" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="13">
+      <c r="C80" s="11">
+        <v>44214</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="12.75">
       <c r="A81" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/meeting-rooms/","Meeting Rooms")</f>
         <v>Meeting Rooms</v>
@@ -1480,7 +1481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="13">
+    <row r="82" spans="1:2" ht="12.75">
       <c r="A82" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/meeting-rooms-ii/","Meeting Rooms II")</f>
         <v>Meeting Rooms II</v>
@@ -1489,7 +1490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="13">
+    <row r="83" spans="1:2" ht="12.75">
       <c r="A83" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/is-subsequence/","Is Subsequence")</f>
         <v>Is Subsequence</v>
@@ -1498,7 +1499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="13">
+    <row r="84" spans="1:2" ht="12.75">
       <c r="A84" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/next-permutation/","Next Permutation")</f>
         <v>Next Permutation</v>
@@ -1507,7 +1508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13">
+    <row r="85" spans="1:2" ht="12.75">
       <c r="A85" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/string-to-integer-atoi/","String to Integer (atoi)")</f>
         <v>String to Integer (atoi)</v>
@@ -1516,7 +1517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="13">
+    <row r="86" spans="1:2" ht="12.75">
       <c r="A86" s="8" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/zigzag-conversion/","ZigZag Conversion")</f>
         <v>ZigZag Conversion</v>
@@ -1546,5 +1547,6 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 83 about LinkedList
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshi\Desktop\leetcode_study\60probrems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A263C-523A-4573-BF3D-24B84D49B256}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F67C44-C1B7-4246-8CD8-810665F8AED6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -202,6 +202,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,10 +227,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -239,8 +247,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="56" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -586,8 +596,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -701,12 +711,18 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="str">
+      <c r="A7" s="15" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/remove-duplicates-from-sorted-list/","Remove Duplicates from Sorted List")</f>
         <v>Remove Duplicates from Sorted List</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C7" s="11">
+        <v>44215</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
add 206 about Stack and LinkedList
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshi\Desktop\leetcode_study\60probrems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F67C44-C1B7-4246-8CD8-810665F8AED6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818D8856-26B7-4006-A16B-2541DBC34F28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -137,12 +137,16 @@
     </rPh>
     <phoneticPr fontId="8"/>
   </si>
+  <si>
+    <t>△</t>
+    <phoneticPr fontId="8"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -209,6 +213,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -248,6 +258,7 @@
     <xf numFmtId="56" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -596,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -770,15 +781,19 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="str">
+      <c r="A13" s="15" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/reverse-linked-list/","Reverse Linked List")</f>
         <v>Reverse Linked List</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="13">
+        <v>44216</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>

</xml_diff>

<commit_message>
add 349 about HashMap
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshi\Desktop\leetcode_study\60probrems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818D8856-26B7-4006-A16B-2541DBC34F28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BD2041-54CF-48AA-89F2-4D62CAB6462B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="31">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -895,6 +895,12 @@
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C23" s="11">
+        <v>44217</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="str">

</xml_diff>

<commit_message>
add 617 about DFS
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5FDDAE-F6F9-B643-B99D-8995554C3F22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DFD26-8727-BC4C-91CD-194E60AF3773}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1047,8 +1047,12 @@
       <c r="B37" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
+      <c r="C37" s="13">
+        <v>44219</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>

</xml_diff>

<commit_message>
add 153 about BinarySearch
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DFD26-8727-BC4C-91CD-194E60AF3773}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B42275-4242-594C-99F5-5CC19662620A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1215,6 +1215,12 @@
       <c r="B53" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C53" s="11">
+        <v>44220</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="54" spans="1:26" ht="13">
       <c r="A54" s="8" t="str">
@@ -1317,6 +1323,12 @@
       <c r="B60" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C60" s="11">
+        <v>44221</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="61" spans="1:26" ht="13">
       <c r="A61" s="8" t="str">

</xml_diff>

<commit_message>
add 2 about LinkedList
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B42275-4242-594C-99F5-5CC19662620A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10AE32-0DA6-3C43-80C5-5CE16AD83156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1376,6 +1376,12 @@
       <c r="B66" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C66" s="11">
+        <v>44222</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="67" spans="1:26" ht="13">
       <c r="A67" s="8" t="str">

</xml_diff>

<commit_message>
add 62 about DP
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10AE32-0DA6-3C43-80C5-5CE16AD83156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB360071-B191-4040-B370-56F49E16DE08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -737,6 +737,12 @@
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="11">
+        <v>44223</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="5"/>
@@ -1449,7 +1455,12 @@
       <c r="B75" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="10"/>
+      <c r="C75" s="11">
+        <v>44224</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>

</xml_diff>

<commit_message>
add 33 about BinarySearch
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC1E8A-3C44-B845-BD6D-360C90176E27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FCDF98-FFE9-504F-BF60-0CEB05F8444F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -890,6 +890,12 @@
       <c r="B24" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C24" s="11">
+        <v>44230</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="str">

</xml_diff>

<commit_message>
add 142 about LinkedList
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FCDF98-FFE9-504F-BF60-0CEB05F8444F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CC64AB-E4DC-C84B-B972-1E9D3D04957D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -710,6 +710,12 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="11">
+        <v>44232</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="str">
@@ -1356,6 +1362,12 @@
       <c r="B61" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C61" s="11">
+        <v>44231</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="62" spans="1:26" ht="13">
       <c r="A62" s="8" t="str">

</xml_diff>

<commit_message>
add 122 and 387
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CC64AB-E4DC-C84B-B972-1E9D3D04957D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0AAD1-5B8D-BB4F-93CE-FB3D000EE923}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1102,6 +1102,12 @@
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C38" s="11">
+        <v>44233</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="str">

</xml_diff>

<commit_message>
add 102 about Tree_BST
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0AAD1-5B8D-BB4F-93CE-FB3D000EE923}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF98B60-782E-3146-99F7-82819613D413}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -725,6 +725,12 @@
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="11">
+        <v>44215</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="str">
@@ -784,8 +790,12 @@
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="13">
+        <v>44216</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -887,6 +897,12 @@
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C23" s="11">
+        <v>44217</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="str">
@@ -910,6 +926,12 @@
       </c>
       <c r="B25" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C25" s="11">
+        <v>44235</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
@@ -1117,6 +1139,12 @@
       <c r="B39" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C39" s="11">
+        <v>44236</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="str">
@@ -1259,6 +1287,12 @@
       </c>
       <c r="B54" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C54" s="11">
+        <v>44235</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="13">

</xml_diff>

<commit_message>
add 347 about Heap
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF98B60-782E-3146-99F7-82819613D413}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF327C41-96A3-F846-AD46-BF66C026FE49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1207,6 +1207,12 @@
       <c r="B47" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C47" s="11">
+        <v>44238</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="48" spans="1:26" ht="13">
       <c r="A48" s="8" t="str">

</xml_diff>

<commit_message>
add 198 about DP
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF327C41-96A3-F846-AD46-BF66C026FE49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B338993-BA46-4049-B71C-C8262866D17A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -850,6 +850,12 @@
       <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C17" s="11">
+        <v>44239</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="str">

</xml_diff>

<commit_message>
add 103 about Tree_BST
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B338993-BA46-4049-B71C-C8262866D17A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150BC5E-3346-D146-8A26-6BC4590306C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1160,6 +1160,12 @@
       <c r="B40" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C40" s="11">
+        <v>44237</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="str">
@@ -1266,6 +1272,12 @@
       </c>
       <c r="B51" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C51" s="11">
+        <v>44240</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="13">

</xml_diff>

<commit_message>
add 82 about LinkedList
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150BC5E-3346-D146-8A26-6BC4590306C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47462FE6-A1DD-8240-A96F-5E3D9406E60A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1175,6 +1175,9 @@
       <c r="B41" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C41" s="11">
+        <v>44241</v>
+      </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="str">
@@ -1679,5 +1682,6 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 98 about Tree_BST
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47462FE6-A1DD-8240-A96F-5E3D9406E60A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2726CDEF-837C-5344-B57D-A302310952ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="30">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -740,6 +740,12 @@
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="11">
+        <v>44247</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="str">
@@ -1267,6 +1273,12 @@
       <c r="B50" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C50" s="11">
+        <v>44248</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="51" spans="1:26" ht="13">
       <c r="A51" s="8" t="str">

</xml_diff>

<commit_message>
add 49 about HashMap
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2726CDEF-837C-5344-B57D-A302310952ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F87A7-BB54-2648-9700-22938EF462C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="31">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -145,6 +145,13 @@
     <t>有料</t>
     <rPh sb="0" eb="2">
       <t>ユウリョ</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>有料</t>
+    <rPh sb="0" eb="2">
+      <t>ユウリョウ</t>
     </rPh>
     <phoneticPr fontId="8"/>
   </si>
@@ -597,8 +604,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1022,6 +1029,9 @@
       <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C31" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="str">
@@ -1193,6 +1203,12 @@
       <c r="B42" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C42" s="11">
+        <v>44250</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="str">

</xml_diff>

<commit_message>
add 39 about Greedy_Backtracking
</commit_message>
<xml_diff>
--- a/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
+++ b/60probrems/60 LeetCode problems to solve for coding interiew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Desktop/leetcode_study/60probrems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F87A7-BB54-2648-9700-22938EF462C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B55FD87-91DF-0940-B379-7DEDE0978FB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="31">
   <si>
     <t>https://leetcode.com/list/xo2bgr0r</t>
   </si>
@@ -604,8 +604,8 @@
   </sheetPr>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -907,6 +907,12 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C22" s="11">
+        <v>44253</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="str">

</xml_diff>